<commit_message>
Nueva edición de las propiedades a desarrollar en el programa
</commit_message>
<xml_diff>
--- a/Fechas de Tareas.xlsx
+++ b/Fechas de Tareas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\Pantera\PruebaPanteraAccedo01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B0CDF3-4207-4E2D-9C72-58056971FAD2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2505EB-7E00-48DA-9F13-096879EE7749}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Tasks</t>
   </si>
@@ -39,16 +39,34 @@
     <t>Fecha de Finalización</t>
   </si>
   <si>
-    <t>Crear input comentario</t>
-  </si>
-  <si>
-    <t>Guardar texto del comentario en la lista de comentarios</t>
-  </si>
-  <si>
-    <t>Recortar imagen seleccionada</t>
-  </si>
-  <si>
-    <t>Agregar imagen</t>
+    <t xml:space="preserve"> 1. Crear input comentario</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2. Guardar texto del comentario en la lista de comentarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3. Agregar imagen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4. Recortar imagen seleccionada</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4.1.  Agregar opción para recortar la imagen seleccionada</t>
+  </si>
+  <si>
+    <t>TERMINADO</t>
+  </si>
+  <si>
+    <t>EN PROCESO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4.2. Agregar la imagen segun la edición de recorte echa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4.3. Agregar modal que selecciona y edite la imagen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5. Agregar estilos</t>
   </si>
 </sst>
 </file>
@@ -94,15 +112,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -110,20 +140,86 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,61 +500,120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="35.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.21875" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.88671875" style="1"/>
     <col min="5" max="5" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="8.88671875" style="1"/>
+    <col min="8" max="8" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4">
+      <c r="F1" s="3">
         <v>45532</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="B2" s="7">
+        <v>45527</v>
+      </c>
+      <c r="C2" s="7">
+        <v>45527</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="B3" s="8">
+        <v>45530</v>
+      </c>
+      <c r="C3" s="8">
+        <v>45530</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="11">
+        <v>45530</v>
+      </c>
+      <c r="C4" s="11">
+        <v>45530</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B5" s="13">
+        <v>45530</v>
+      </c>
+      <c r="C5" s="13">
+        <v>45531</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+    </row>
+    <row r="7" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+    </row>
+    <row r="8" spans="1:9" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+    </row>
+    <row r="9" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Detalle adicional del documento "Fechas de Tareas"
</commit_message>
<xml_diff>
--- a/Fechas de Tareas.xlsx
+++ b/Fechas de Tareas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\Pantera\PruebaPanteraAccedo01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2505EB-7E00-48DA-9F13-096879EE7749}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07081924-9B6B-4A63-96A3-A794DF740512}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -173,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -203,23 +203,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,7 +512,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -521,13 +530,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="16" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -580,42 +589,46 @@
       <c r="A5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="20">
         <v>45530</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="17">
         <v>45531</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="18"/>
     </row>
     <row r="7" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="18"/>
     </row>
     <row r="8" spans="1:9" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="19"/>
     </row>
     <row r="9" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="C5:C8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
- Funciones iniciales. - Reajuste de los elementos Html.
</commit_message>
<xml_diff>
--- a/Fechas de Tareas.xlsx
+++ b/Fechas de Tareas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\Pantera\PruebaPanteraAccedo01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07081924-9B6B-4A63-96A3-A794DF740512}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A11FFC52-9DAC-4B29-9E2F-00DA32164520}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -173,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -211,15 +211,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -228,6 +220,15 @@
     </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -512,7 +513,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -589,10 +590,10 @@
       <c r="A5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="18">
         <v>45530</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="21">
         <v>45531</v>
       </c>
     </row>
@@ -600,29 +601,33 @@
       <c r="A6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="18"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="22"/>
     </row>
     <row r="7" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="18"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="22"/>
     </row>
     <row r="8" spans="1:9" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="23"/>
     </row>
     <row r="9" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
+      <c r="B9" s="17">
+        <v>45531</v>
+      </c>
+      <c r="C9" s="17">
+        <v>45531</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Edición del archivo Excel
</commit_message>
<xml_diff>
--- a/Fechas de Tareas.xlsx
+++ b/Fechas de Tareas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\Pantera\PruebaPanteraAccedo01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A11FFC52-9DAC-4B29-9E2F-00DA32164520}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D41036D-D7F0-46D9-9D00-D0B2AF25E6CB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="14">
   <si>
     <t>Tasks</t>
   </si>
@@ -191,43 +191,43 @@
     <xf numFmtId="16" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -513,7 +513,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C4"/>
+      <selection activeCell="A5" sqref="A5:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -531,13 +531,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -565,67 +565,67 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="11">
         <v>45530</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="11">
         <v>45530</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="8">
         <v>45530</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="8">
         <v>45530</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="16">
         <v>45530</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="17">
         <v>45531</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="19"/>
-      <c r="C6" s="22"/>
+      <c r="C6" s="20"/>
     </row>
     <row r="7" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="18" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="19"/>
-      <c r="C7" s="22"/>
+      <c r="C7" s="20"/>
     </row>
     <row r="8" spans="1:9" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="20"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="23"/>
     </row>
     <row r="9" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="13">
         <v>45531</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="13">
         <v>45531</v>
       </c>
     </row>

</xml_diff>